<commit_message>
fixed halved freq issue + updated doc
</commit_message>
<xml_diff>
--- a/doc/dma_pwm_pulse_width_calculator.xlsx
+++ b/doc/dma_pwm_pulse_width_calculator.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ben\Documents\RT Robot\Documentation\Topics\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ben\Documents\Projects\RT Robot\Documentation\Topics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02031A9A-64A4-4FA6-BB58-FA5618841A14}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B4D5F0A-1325-41DC-B27E-13C1AAB46A87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4515" yWindow="2640" windowWidth="30540" windowHeight="17895" xr2:uid="{581135D7-DF17-4593-87AB-39E2EE409C02}"/>
+    <workbookView xWindow="23940" yWindow="630" windowWidth="30195" windowHeight="14730" xr2:uid="{581135D7-DF17-4593-87AB-39E2EE409C02}"/>
   </bookViews>
   <sheets>
     <sheet name="Pulse Width" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,10 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -88,7 +91,7 @@
     <t>DMA PWM Pulse Width Calculator</t>
   </si>
   <si>
-    <t>Version 1.0</t>
+    <t>Version 2.0</t>
   </si>
 </sst>
 </file>
@@ -211,7 +214,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -232,9 +235,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -245,11 +245,14 @@
     <xf numFmtId="3" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="11" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -257,14 +260,17 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -583,7 +589,7 @@
   <dimension ref="B1:P19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:K3"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -608,30 +614,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
     </row>
     <row r="2" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="19" t="s">
+      <c r="B2" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="19"/>
-      <c r="G2" s="19"/>
-      <c r="H2" s="19"/>
-      <c r="I2" s="19"/>
-      <c r="J2" s="19"/>
-      <c r="K2" s="19"/>
-      <c r="L2" s="13" t="s">
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="17"/>
+      <c r="H2" s="17"/>
+      <c r="I2" s="17"/>
+      <c r="J2" s="17"/>
+      <c r="K2" s="17"/>
+      <c r="L2" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="M2" s="13"/>
-      <c r="N2" s="13"/>
-      <c r="O2" s="13"/>
-      <c r="P2" s="13"/>
+      <c r="M2" s="19"/>
+      <c r="N2" s="19"/>
+      <c r="O2" s="19"/>
+      <c r="P2" s="19"/>
     </row>
     <row r="3" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="18"/>
@@ -644,19 +650,18 @@
       <c r="I3" s="18"/>
       <c r="J3" s="18"/>
       <c r="K3" s="18"/>
-      <c r="L3" s="14"/>
-      <c r="M3" s="14"/>
-      <c r="N3" s="14"/>
-      <c r="O3" s="14"/>
-      <c r="P3" s="14"/>
+      <c r="L3" s="20"/>
+      <c r="M3" s="20"/>
+      <c r="N3" s="20"/>
+      <c r="O3" s="20"/>
+      <c r="P3" s="20"/>
     </row>
     <row r="5" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="7">
-        <f>0.000001</f>
-        <v>9.9999999999999995E-7</v>
+      <c r="C5" s="13">
+        <v>1.0000000000000001E-5</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>4</v>
@@ -669,17 +674,17 @@
         <v>15</v>
       </c>
       <c r="I5" s="16"/>
-      <c r="J5" s="17" t="s">
+      <c r="J5" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="K5" s="17" t="s">
+      <c r="K5" s="12" t="s">
         <v>14</v>
       </c>
       <c r="L5" s="15" t="s">
         <v>12</v>
       </c>
       <c r="M5" s="16"/>
-      <c r="N5" s="17" t="s">
+      <c r="N5" s="12" t="s">
         <v>5</v>
       </c>
       <c r="O5" s="15" t="s">
@@ -691,7 +696,7 @@
       <c r="B6" s="1"/>
       <c r="C6" s="1">
         <f>C5*10^6</f>
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>2</v>
@@ -710,36 +715,36 @@
         <v>4</v>
       </c>
       <c r="J6" s="3">
-        <f>_xlfn.FLOOR.MATH(H6/$C$5)</f>
-        <v>20000000</v>
+        <f>_xlfn.FLOOR.MATH(H6/$C$5/2)</f>
+        <v>1000000</v>
       </c>
       <c r="K6" s="5">
         <f t="shared" ref="K6:K7" si="1">(1-(J6-1)/J6)</f>
-        <v>5.0000000029193359E-8</v>
+        <v>1.0000000000287557E-6</v>
       </c>
       <c r="L6" s="3">
         <f t="shared" ref="L6:L7" si="2">J6*32</f>
-        <v>640000000</v>
+        <v>32000000</v>
       </c>
       <c r="M6" s="3" t="s">
         <v>6</v>
       </c>
       <c r="N6" s="3">
         <f t="shared" ref="N6:N7" si="3">_xlfn.CEILING.MATH(L6/4096)</f>
-        <v>156250</v>
+        <v>7813</v>
       </c>
       <c r="O6" s="3">
-        <f>1/($C$5*J6)</f>
-        <v>0.05</v>
+        <f t="shared" ref="O6:O19" si="4">1/($C$5*J6)</f>
+        <v>0.1</v>
       </c>
       <c r="P6" s="3" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="7" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B7" s="10"/>
-      <c r="C7" s="10"/>
-      <c r="D7" s="10"/>
+      <c r="B7" s="9"/>
+      <c r="C7" s="9"/>
+      <c r="D7" s="9"/>
       <c r="F7" s="3">
         <v>0.1</v>
       </c>
@@ -754,124 +759,124 @@
         <v>4</v>
       </c>
       <c r="J7" s="3">
-        <f>_xlfn.FLOOR.MATH(H7/$C$5)</f>
-        <v>10000000</v>
+        <f t="shared" ref="J7:J19" si="5">_xlfn.FLOOR.MATH(H7/$C$5/2)</f>
+        <v>500000</v>
       </c>
       <c r="K7" s="5">
         <f t="shared" si="1"/>
-        <v>9.9999999947364415E-8</v>
+        <v>1.999999999946489E-6</v>
       </c>
       <c r="L7" s="3">
         <f t="shared" si="2"/>
-        <v>320000000</v>
+        <v>16000000</v>
       </c>
       <c r="M7" s="3" t="s">
         <v>6</v>
       </c>
       <c r="N7" s="3">
         <f t="shared" si="3"/>
-        <v>78125</v>
+        <v>3907</v>
       </c>
       <c r="O7" s="3">
-        <f>1/($C$5*J7)</f>
+        <f t="shared" si="4"/>
+        <v>0.2</v>
+      </c>
+      <c r="P7" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B8" s="9"/>
+      <c r="C8" s="9"/>
+      <c r="D8" s="9"/>
+      <c r="F8" s="3">
+        <v>1</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="H8" s="4">
+        <f t="shared" ref="H8:H16" si="6">1/F8</f>
+        <v>1</v>
+      </c>
+      <c r="I8" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="J8" s="3">
+        <f t="shared" si="5"/>
+        <v>50000</v>
+      </c>
+      <c r="K8" s="5">
+        <f t="shared" ref="K8:K16" si="7">(1-(J8-1)/J8)</f>
+        <v>2.0000000000020002E-5</v>
+      </c>
+      <c r="L8" s="3">
+        <f t="shared" ref="L8:L16" si="8">J8*32</f>
+        <v>1600000</v>
+      </c>
+      <c r="M8" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="N8" s="3">
+        <f t="shared" ref="N8:N16" si="9">_xlfn.CEILING.MATH(L8/4096)</f>
+        <v>391</v>
+      </c>
+      <c r="O8" s="3">
+        <f t="shared" si="4"/>
+        <v>2</v>
+      </c>
+      <c r="P8" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B9" s="9"/>
+      <c r="C9" s="10"/>
+      <c r="D9" s="9"/>
+      <c r="F9" s="3">
+        <v>10</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="H9" s="4">
+        <f t="shared" si="6"/>
         <v>0.1</v>
       </c>
-      <c r="P7" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B8" s="10"/>
-      <c r="C8" s="10"/>
-      <c r="D8" s="10"/>
-      <c r="F8" s="3">
-        <v>1</v>
-      </c>
-      <c r="G8" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="H8" s="4">
-        <f t="shared" ref="H8:H16" si="4">1/F8</f>
-        <v>1</v>
-      </c>
-      <c r="I8" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="J8" s="3">
-        <f>_xlfn.FLOOR.MATH(H8/$C$5)</f>
-        <v>1000000</v>
-      </c>
-      <c r="K8" s="5">
-        <f t="shared" ref="K8:K16" si="5">(1-(J8-1)/J8)</f>
-        <v>1.0000000000287557E-6</v>
-      </c>
-      <c r="L8" s="3">
-        <f t="shared" ref="L8:L16" si="6">J8*32</f>
-        <v>32000000</v>
-      </c>
-      <c r="M8" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="N8" s="3">
-        <f t="shared" ref="N8:N16" si="7">_xlfn.CEILING.MATH(L8/4096)</f>
-        <v>7813</v>
-      </c>
-      <c r="O8" s="3">
-        <f>1/($C$5*J8)</f>
-        <v>1</v>
-      </c>
-      <c r="P8" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="9" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B9" s="10"/>
-      <c r="C9" s="11"/>
-      <c r="D9" s="10"/>
-      <c r="F9" s="3">
-        <v>10</v>
-      </c>
-      <c r="G9" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="H9" s="4">
-        <f t="shared" si="4"/>
-        <v>0.1</v>
-      </c>
       <c r="I9" s="3" t="s">
         <v>4</v>
       </c>
       <c r="J9" s="3">
-        <f>_xlfn.FLOOR.MATH(H9/$C$5)</f>
-        <v>100000</v>
+        <f t="shared" si="5"/>
+        <v>5000</v>
       </c>
       <c r="K9" s="5">
-        <f t="shared" si="5"/>
-        <v>9.9999999999544897E-6</v>
+        <f t="shared" si="7"/>
+        <v>1.9999999999997797E-4</v>
       </c>
       <c r="L9" s="3">
-        <f t="shared" si="6"/>
-        <v>3200000</v>
+        <f t="shared" si="8"/>
+        <v>160000</v>
       </c>
       <c r="M9" s="3" t="s">
         <v>6</v>
       </c>
       <c r="N9" s="3">
-        <f t="shared" si="7"/>
-        <v>782</v>
+        <f t="shared" si="9"/>
+        <v>40</v>
       </c>
       <c r="O9" s="3">
-        <f>1/($C$5*J9)</f>
-        <v>10</v>
+        <f t="shared" si="4"/>
+        <v>20</v>
       </c>
       <c r="P9" s="3" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="10" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B10" s="10"/>
-      <c r="C10" s="10"/>
-      <c r="D10" s="10"/>
+      <c r="B10" s="9"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="9"/>
       <c r="F10" s="3">
         <v>50</v>
       </c>
@@ -879,34 +884,34 @@
         <v>3</v>
       </c>
       <c r="H10" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0.02</v>
       </c>
       <c r="I10" s="3" t="s">
         <v>4</v>
       </c>
       <c r="J10" s="3">
-        <f>_xlfn.FLOOR.MATH(H10/$C$5)</f>
-        <v>20000</v>
+        <f t="shared" si="5"/>
+        <v>1000</v>
       </c>
       <c r="K10" s="5">
-        <f t="shared" si="5"/>
-        <v>4.9999999999994493E-5</v>
+        <f t="shared" si="7"/>
+        <v>1.0000000000000009E-3</v>
       </c>
       <c r="L10" s="3">
-        <f t="shared" si="6"/>
-        <v>640000</v>
+        <f t="shared" si="8"/>
+        <v>32000</v>
       </c>
       <c r="M10" s="3" t="s">
         <v>6</v>
       </c>
       <c r="N10" s="3">
-        <f t="shared" si="7"/>
-        <v>157</v>
+        <f t="shared" si="9"/>
+        <v>8</v>
       </c>
       <c r="O10" s="3">
-        <f>1/($C$5*J10)</f>
-        <v>50</v>
+        <f t="shared" si="4"/>
+        <v>100</v>
       </c>
       <c r="P10" s="3" t="s">
         <v>10</v>
@@ -923,34 +928,34 @@
         <v>3</v>
       </c>
       <c r="H11" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0.01</v>
       </c>
       <c r="I11" s="3" t="s">
         <v>4</v>
       </c>
       <c r="J11" s="3">
-        <f>_xlfn.FLOOR.MATH(H11/$C$5)</f>
-        <v>10000</v>
+        <f t="shared" si="5"/>
+        <v>500</v>
       </c>
       <c r="K11" s="5">
-        <f t="shared" si="5"/>
-        <v>9.9999999999988987E-5</v>
+        <f t="shared" si="7"/>
+        <v>2.0000000000000018E-3</v>
       </c>
       <c r="L11" s="3">
-        <f t="shared" si="6"/>
-        <v>320000</v>
+        <f t="shared" si="8"/>
+        <v>16000</v>
       </c>
       <c r="M11" s="3" t="s">
         <v>6</v>
       </c>
       <c r="N11" s="3">
-        <f t="shared" si="7"/>
-        <v>79</v>
+        <f t="shared" si="9"/>
+        <v>4</v>
       </c>
       <c r="O11" s="3">
-        <f>1/($C$5*J11)</f>
-        <v>100</v>
+        <f t="shared" si="4"/>
+        <v>200</v>
       </c>
       <c r="P11" s="3" t="s">
         <v>10</v>
@@ -964,34 +969,34 @@
         <v>3</v>
       </c>
       <c r="H12" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>1E-3</v>
       </c>
       <c r="I12" s="3" t="s">
         <v>4</v>
       </c>
       <c r="J12" s="3">
-        <f>_xlfn.FLOOR.MATH(H12/$C$5)</f>
-        <v>1000</v>
+        <f t="shared" si="5"/>
+        <v>50</v>
       </c>
       <c r="K12" s="5">
-        <f t="shared" si="5"/>
-        <v>1.0000000000000009E-3</v>
+        <f t="shared" si="7"/>
+        <v>2.0000000000000018E-2</v>
       </c>
       <c r="L12" s="3">
-        <f t="shared" si="6"/>
-        <v>32000</v>
+        <f t="shared" si="8"/>
+        <v>1600</v>
       </c>
       <c r="M12" s="3" t="s">
         <v>6</v>
       </c>
       <c r="N12" s="3">
-        <f t="shared" si="7"/>
-        <v>8</v>
+        <f t="shared" si="9"/>
+        <v>1</v>
       </c>
       <c r="O12" s="3">
-        <f>1/($C$5*J12)</f>
-        <v>1000</v>
+        <f t="shared" si="4"/>
+        <v>2000</v>
       </c>
       <c r="P12" s="3" t="s">
         <v>10</v>
@@ -1005,34 +1010,34 @@
         <v>3</v>
       </c>
       <c r="H13" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>2.0000000000000001E-4</v>
       </c>
       <c r="I13" s="3" t="s">
         <v>4</v>
       </c>
       <c r="J13" s="3">
-        <f>_xlfn.FLOOR.MATH(H13/$C$5)</f>
-        <v>200</v>
+        <f t="shared" si="5"/>
+        <v>10</v>
       </c>
       <c r="K13" s="5">
-        <f t="shared" si="5"/>
-        <v>5.0000000000000044E-3</v>
+        <f t="shared" si="7"/>
+        <v>9.9999999999999978E-2</v>
       </c>
       <c r="L13" s="3">
-        <f t="shared" si="6"/>
-        <v>6400</v>
+        <f t="shared" si="8"/>
+        <v>320</v>
       </c>
       <c r="M13" s="3" t="s">
         <v>6</v>
       </c>
       <c r="N13" s="3">
-        <f t="shared" si="7"/>
-        <v>2</v>
+        <f t="shared" si="9"/>
+        <v>1</v>
       </c>
       <c r="O13" s="3">
-        <f>1/($C$5*J13)</f>
-        <v>5000</v>
+        <f t="shared" si="4"/>
+        <v>10000</v>
       </c>
       <c r="P13" s="3" t="s">
         <v>10</v>
@@ -1046,34 +1051,34 @@
         <v>3</v>
       </c>
       <c r="H14" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>1E-4</v>
       </c>
       <c r="I14" s="3" t="s">
         <v>4</v>
       </c>
       <c r="J14" s="3">
-        <f>_xlfn.FLOOR.MATH(H14/$C$5)</f>
-        <v>100</v>
+        <f t="shared" si="5"/>
+        <v>5</v>
       </c>
       <c r="K14" s="5">
-        <f t="shared" si="5"/>
-        <v>1.0000000000000009E-2</v>
+        <f t="shared" si="7"/>
+        <v>0.19999999999999996</v>
       </c>
       <c r="L14" s="3">
-        <f t="shared" si="6"/>
-        <v>3200</v>
+        <f t="shared" si="8"/>
+        <v>160</v>
       </c>
       <c r="M14" s="3" t="s">
         <v>6</v>
       </c>
       <c r="N14" s="3">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="O14" s="3">
-        <f>1/($C$5*J14)</f>
-        <v>10000</v>
+        <f t="shared" si="4"/>
+        <v>20000</v>
       </c>
       <c r="P14" s="3" t="s">
         <v>10</v>
@@ -1087,34 +1092,34 @@
         <v>3</v>
       </c>
       <c r="H15" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>5.5555555555555558E-5</v>
       </c>
       <c r="I15" s="3" t="s">
         <v>4</v>
       </c>
       <c r="J15" s="3">
-        <f>_xlfn.FLOOR.MATH(H15/$C$5)</f>
-        <v>55</v>
+        <f t="shared" si="5"/>
+        <v>2</v>
       </c>
       <c r="K15" s="5">
-        <f t="shared" si="5"/>
-        <v>1.8181818181818188E-2</v>
+        <f t="shared" si="7"/>
+        <v>0.5</v>
       </c>
       <c r="L15" s="3">
-        <f t="shared" si="6"/>
-        <v>1760</v>
+        <f t="shared" si="8"/>
+        <v>64</v>
       </c>
       <c r="M15" s="3" t="s">
         <v>6</v>
       </c>
       <c r="N15" s="3">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="O15" s="3">
-        <f>1/($C$5*J15)</f>
-        <v>18181.818181818184</v>
+        <f t="shared" si="4"/>
+        <v>49999.999999999993</v>
       </c>
       <c r="P15" s="3" t="s">
         <v>10</v>
@@ -1128,34 +1133,34 @@
         <v>3</v>
       </c>
       <c r="H16" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>5.0000000000000002E-5</v>
       </c>
       <c r="I16" s="3" t="s">
         <v>4</v>
       </c>
       <c r="J16" s="3">
-        <f>_xlfn.FLOOR.MATH(H16/$C$5)</f>
-        <v>50</v>
+        <f t="shared" si="5"/>
+        <v>2</v>
       </c>
       <c r="K16" s="5">
-        <f t="shared" si="5"/>
-        <v>2.0000000000000018E-2</v>
+        <f t="shared" si="7"/>
+        <v>0.5</v>
       </c>
       <c r="L16" s="3">
-        <f t="shared" si="6"/>
-        <v>1600</v>
+        <f t="shared" si="8"/>
+        <v>64</v>
       </c>
       <c r="M16" s="3" t="s">
         <v>6</v>
       </c>
       <c r="N16" s="3">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="O16" s="3">
-        <f>1/($C$5*J16)</f>
-        <v>20000</v>
+        <f t="shared" si="4"/>
+        <v>49999.999999999993</v>
       </c>
       <c r="P16" s="3" t="s">
         <v>10</v>
@@ -1169,34 +1174,34 @@
         <v>3</v>
       </c>
       <c r="H17" s="4">
-        <f t="shared" ref="H17:H19" si="8">1/F17</f>
+        <f t="shared" ref="H17:H19" si="10">1/F17</f>
         <v>2.0000000000000002E-5</v>
       </c>
       <c r="I17" s="3" t="s">
         <v>4</v>
       </c>
       <c r="J17" s="3">
-        <f>_xlfn.FLOOR.MATH(H17/$C$5)</f>
-        <v>20</v>
+        <f t="shared" si="5"/>
+        <v>1</v>
       </c>
       <c r="K17" s="5">
-        <f t="shared" ref="K17:K19" si="9">(1-(J17-1)/J17)</f>
-        <v>5.0000000000000044E-2</v>
+        <f t="shared" ref="K17:K19" si="11">(1-(J17-1)/J17)</f>
+        <v>1</v>
       </c>
       <c r="L17" s="3">
-        <f t="shared" ref="L17:L19" si="10">J17*32</f>
-        <v>640</v>
+        <f t="shared" ref="L17:L19" si="12">J17*32</f>
+        <v>32</v>
       </c>
       <c r="M17" s="3" t="s">
         <v>6</v>
       </c>
       <c r="N17" s="3">
-        <f t="shared" ref="N17:N19" si="11">_xlfn.CEILING.MATH(L17/4096)</f>
+        <f t="shared" ref="N17:N19" si="13">_xlfn.CEILING.MATH(L17/4096)</f>
         <v>1</v>
       </c>
       <c r="O17" s="3">
-        <f>1/($C$5*J17)</f>
-        <v>50000.000000000007</v>
+        <f t="shared" si="4"/>
+        <v>99999.999999999985</v>
       </c>
       <c r="P17" s="3" t="s">
         <v>10</v>
@@ -1210,34 +1215,34 @@
         <v>3</v>
       </c>
       <c r="H18" s="4">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>1.0000000000000001E-5</v>
       </c>
       <c r="I18" s="3" t="s">
         <v>4</v>
       </c>
       <c r="J18" s="3">
-        <f>_xlfn.FLOOR.MATH(H18/$C$5)</f>
-        <v>10</v>
-      </c>
-      <c r="K18" s="5">
-        <f t="shared" si="9"/>
-        <v>9.9999999999999978E-2</v>
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="K18" s="5" t="e">
+        <f t="shared" si="11"/>
+        <v>#DIV/0!</v>
       </c>
       <c r="L18" s="3">
-        <f t="shared" si="10"/>
-        <v>320</v>
+        <f t="shared" si="12"/>
+        <v>0</v>
       </c>
       <c r="M18" s="3" t="s">
         <v>6</v>
       </c>
       <c r="N18" s="3">
-        <f t="shared" si="11"/>
-        <v>1</v>
-      </c>
-      <c r="O18" s="3">
-        <f>1/($C$5*J18)</f>
-        <v>100000.00000000001</v>
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="O18" s="3" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
       </c>
       <c r="P18" s="3" t="s">
         <v>10</v>
@@ -1251,34 +1256,34 @@
         <v>3</v>
       </c>
       <c r="H19" s="4">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>1.9999999999999999E-6</v>
       </c>
       <c r="I19" s="3" t="s">
         <v>4</v>
       </c>
       <c r="J19" s="3">
-        <f>_xlfn.FLOOR.MATH(H19/$C$5)</f>
-        <v>2</v>
-      </c>
-      <c r="K19" s="5">
-        <f t="shared" si="9"/>
-        <v>0.5</v>
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="K19" s="5" t="e">
+        <f t="shared" si="11"/>
+        <v>#DIV/0!</v>
       </c>
       <c r="L19" s="3">
-        <f t="shared" si="10"/>
-        <v>64</v>
+        <f t="shared" si="12"/>
+        <v>0</v>
       </c>
       <c r="M19" s="3" t="s">
         <v>6</v>
       </c>
       <c r="N19" s="3">
-        <f t="shared" si="11"/>
-        <v>1</v>
-      </c>
-      <c r="O19" s="3">
-        <f>1/($C$5*J19)</f>
-        <v>500000</v>
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="O19" s="3" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
       </c>
       <c r="P19" s="3" t="s">
         <v>10</v>
@@ -1303,7 +1308,7 @@
   <dimension ref="B2:P19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1328,25 +1333,25 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B2" s="19" t="s">
+      <c r="B2" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="19"/>
-      <c r="G2" s="19"/>
-      <c r="H2" s="19"/>
-      <c r="I2" s="19"/>
-      <c r="J2" s="19"/>
-      <c r="K2" s="19"/>
-      <c r="L2" s="13" t="s">
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="17"/>
+      <c r="H2" s="17"/>
+      <c r="I2" s="17"/>
+      <c r="J2" s="17"/>
+      <c r="K2" s="17"/>
+      <c r="L2" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="M2" s="13"/>
-      <c r="N2" s="13"/>
-      <c r="O2" s="13"/>
-      <c r="P2" s="13"/>
+      <c r="M2" s="19"/>
+      <c r="N2" s="19"/>
+      <c r="O2" s="19"/>
+      <c r="P2" s="19"/>
     </row>
     <row r="3" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B3" s="18"/>
@@ -1359,11 +1364,11 @@
       <c r="I3" s="18"/>
       <c r="J3" s="18"/>
       <c r="K3" s="18"/>
-      <c r="L3" s="14"/>
-      <c r="M3" s="14"/>
-      <c r="N3" s="14"/>
-      <c r="O3" s="14"/>
-      <c r="P3" s="14"/>
+      <c r="L3" s="20"/>
+      <c r="M3" s="20"/>
+      <c r="N3" s="20"/>
+      <c r="O3" s="20"/>
+      <c r="P3" s="20"/>
     </row>
     <row r="5" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
@@ -1383,17 +1388,17 @@
         <v>15</v>
       </c>
       <c r="I5" s="16"/>
-      <c r="J5" s="17" t="s">
+      <c r="J5" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="K5" s="17" t="s">
+      <c r="K5" s="12" t="s">
         <v>14</v>
       </c>
       <c r="L5" s="15" t="s">
         <v>12</v>
       </c>
       <c r="M5" s="16"/>
-      <c r="N5" s="17" t="s">
+      <c r="N5" s="12" t="s">
         <v>5</v>
       </c>
       <c r="O5" s="15" t="s">
@@ -1423,27 +1428,27 @@
         <v>4</v>
       </c>
       <c r="J6" s="3">
-        <f>_xlfn.FLOOR.MATH(H6/$C$12)</f>
-        <v>20000000</v>
+        <f>_xlfn.FLOOR.MATH(H6/$C$12/2)</f>
+        <v>1000000</v>
       </c>
       <c r="K6" s="5">
         <f t="shared" ref="K6:K19" si="1">(1-(J6-1)/J6)</f>
-        <v>5.0000000029193359E-8</v>
+        <v>1.0000000000287557E-6</v>
       </c>
       <c r="L6" s="3">
         <f t="shared" ref="L6:L19" si="2">J6*32</f>
-        <v>640000000</v>
+        <v>32000000</v>
       </c>
       <c r="M6" s="3" t="s">
         <v>6</v>
       </c>
       <c r="N6" s="3">
         <f t="shared" ref="N6:N19" si="3">_xlfn.CEILING.MATH(L6/4096)</f>
-        <v>156250</v>
+        <v>7813</v>
       </c>
       <c r="O6" s="3">
-        <f>1/($C$12*J6)</f>
-        <v>0.05</v>
+        <f t="shared" ref="O6:O19" si="4">1/($C$12*J6)</f>
+        <v>0.1</v>
       </c>
       <c r="P6" s="3" t="s">
         <v>10</v>
@@ -1467,27 +1472,27 @@
         <v>4</v>
       </c>
       <c r="J7" s="3">
-        <f>_xlfn.FLOOR.MATH(H7/$C$12)</f>
-        <v>10000000</v>
+        <f t="shared" ref="J7:J19" si="5">_xlfn.FLOOR.MATH(H7/$C$12/2)</f>
+        <v>500000</v>
       </c>
       <c r="K7" s="5">
         <f t="shared" si="1"/>
-        <v>9.9999999947364415E-8</v>
+        <v>1.999999999946489E-6</v>
       </c>
       <c r="L7" s="3">
         <f t="shared" si="2"/>
-        <v>320000000</v>
+        <v>16000000</v>
       </c>
       <c r="M7" s="3" t="s">
         <v>6</v>
       </c>
       <c r="N7" s="3">
         <f t="shared" si="3"/>
-        <v>78125</v>
+        <v>3907</v>
       </c>
       <c r="O7" s="3">
-        <f>1/($C$12*J7)</f>
-        <v>0.1</v>
+        <f t="shared" si="4"/>
+        <v>0.2</v>
       </c>
       <c r="P7" s="3" t="s">
         <v>10</v>
@@ -1518,27 +1523,27 @@
         <v>4</v>
       </c>
       <c r="J8" s="3">
-        <f>_xlfn.FLOOR.MATH(H8/$C$12)</f>
-        <v>1000000</v>
+        <f t="shared" si="5"/>
+        <v>50000</v>
       </c>
       <c r="K8" s="5">
         <f t="shared" si="1"/>
-        <v>1.0000000000287557E-6</v>
+        <v>2.0000000000020002E-5</v>
       </c>
       <c r="L8" s="3">
         <f t="shared" si="2"/>
-        <v>32000000</v>
+        <v>1600000</v>
       </c>
       <c r="M8" s="3" t="s">
         <v>6</v>
       </c>
       <c r="N8" s="3">
         <f t="shared" si="3"/>
-        <v>7813</v>
+        <v>391</v>
       </c>
       <c r="O8" s="3">
-        <f>1/($C$12*J8)</f>
-        <v>1</v>
+        <f t="shared" si="4"/>
+        <v>2</v>
       </c>
       <c r="P8" s="3" t="s">
         <v>10</v>
@@ -1548,8 +1553,8 @@
       <c r="B9" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="12">
-        <v>10</v>
+      <c r="C9" s="11">
+        <v>100</v>
       </c>
       <c r="D9" s="1"/>
       <c r="F9" s="3">
@@ -1566,27 +1571,27 @@
         <v>4</v>
       </c>
       <c r="J9" s="3">
-        <f>_xlfn.FLOOR.MATH(H9/$C$12)</f>
-        <v>100000</v>
+        <f t="shared" si="5"/>
+        <v>5000</v>
       </c>
       <c r="K9" s="5">
         <f t="shared" si="1"/>
-        <v>9.9999999999544897E-6</v>
+        <v>1.9999999999997797E-4</v>
       </c>
       <c r="L9" s="3">
         <f t="shared" si="2"/>
-        <v>3200000</v>
+        <v>160000</v>
       </c>
       <c r="M9" s="3" t="s">
         <v>6</v>
       </c>
       <c r="N9" s="3">
         <f t="shared" si="3"/>
-        <v>782</v>
+        <v>40</v>
       </c>
       <c r="O9" s="3">
-        <f>1/($C$12*J9)</f>
-        <v>10</v>
+        <f t="shared" si="4"/>
+        <v>20</v>
       </c>
       <c r="P9" s="3" t="s">
         <v>10</v>
@@ -1610,27 +1615,27 @@
         <v>4</v>
       </c>
       <c r="J10" s="3">
-        <f>_xlfn.FLOOR.MATH(H10/$C$12)</f>
-        <v>20000</v>
+        <f t="shared" si="5"/>
+        <v>1000</v>
       </c>
       <c r="K10" s="5">
         <f t="shared" si="1"/>
-        <v>4.9999999999994493E-5</v>
+        <v>1.0000000000000009E-3</v>
       </c>
       <c r="L10" s="3">
         <f t="shared" si="2"/>
-        <v>640000</v>
+        <v>32000</v>
       </c>
       <c r="M10" s="3" t="s">
         <v>6</v>
       </c>
       <c r="N10" s="3">
         <f t="shared" si="3"/>
-        <v>157</v>
+        <v>8</v>
       </c>
       <c r="O10" s="3">
-        <f>1/($C$12*J10)</f>
-        <v>50</v>
+        <f t="shared" si="4"/>
+        <v>100</v>
       </c>
       <c r="P10" s="3" t="s">
         <v>10</v>
@@ -1654,27 +1659,27 @@
         <v>4</v>
       </c>
       <c r="J11" s="3">
-        <f>_xlfn.FLOOR.MATH(H11/$C$12)</f>
-        <v>10000</v>
+        <f t="shared" si="5"/>
+        <v>500</v>
       </c>
       <c r="K11" s="5">
         <f t="shared" si="1"/>
-        <v>9.9999999999988987E-5</v>
+        <v>2.0000000000000018E-3</v>
       </c>
       <c r="L11" s="3">
         <f t="shared" si="2"/>
-        <v>320000</v>
+        <v>16000</v>
       </c>
       <c r="M11" s="3" t="s">
         <v>6</v>
       </c>
       <c r="N11" s="3">
         <f t="shared" si="3"/>
-        <v>79</v>
+        <v>4</v>
       </c>
       <c r="O11" s="3">
-        <f>1/($C$12*J11)</f>
-        <v>100</v>
+        <f t="shared" si="4"/>
+        <v>200</v>
       </c>
       <c r="P11" s="3" t="s">
         <v>10</v>
@@ -1684,9 +1689,9 @@
       <c r="B12" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C12" s="8">
+      <c r="C12" s="14">
         <f>C9/(C8*10^6)</f>
-        <v>9.9999999999999995E-7</v>
+        <v>1.0000000000000001E-5</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>4</v>
@@ -1705,27 +1710,27 @@
         <v>4</v>
       </c>
       <c r="J12" s="3">
-        <f>_xlfn.FLOOR.MATH(H12/$C$12)</f>
-        <v>1000</v>
+        <f t="shared" si="5"/>
+        <v>50</v>
       </c>
       <c r="K12" s="5">
         <f t="shared" si="1"/>
-        <v>1.0000000000000009E-3</v>
+        <v>2.0000000000000018E-2</v>
       </c>
       <c r="L12" s="3">
         <f t="shared" si="2"/>
-        <v>32000</v>
+        <v>1600</v>
       </c>
       <c r="M12" s="3" t="s">
         <v>6</v>
       </c>
       <c r="N12" s="3">
         <f t="shared" si="3"/>
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="O12" s="3">
-        <f>1/($C$12*J12)</f>
-        <v>1000</v>
+        <f t="shared" si="4"/>
+        <v>2000</v>
       </c>
       <c r="P12" s="3" t="s">
         <v>10</v>
@@ -1735,7 +1740,7 @@
       <c r="B13" s="1"/>
       <c r="C13" s="1">
         <f>C12*10^6</f>
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>2</v>
@@ -1754,27 +1759,27 @@
         <v>4</v>
       </c>
       <c r="J13" s="3">
-        <f>_xlfn.FLOOR.MATH(H13/$C$12)</f>
-        <v>200</v>
+        <f t="shared" si="5"/>
+        <v>10</v>
       </c>
       <c r="K13" s="5">
         <f t="shared" si="1"/>
-        <v>5.0000000000000044E-3</v>
+        <v>9.9999999999999978E-2</v>
       </c>
       <c r="L13" s="3">
         <f t="shared" si="2"/>
-        <v>6400</v>
+        <v>320</v>
       </c>
       <c r="M13" s="3" t="s">
         <v>6</v>
       </c>
       <c r="N13" s="3">
         <f t="shared" si="3"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="O13" s="3">
-        <f>1/($C$12*J13)</f>
-        <v>5000</v>
+        <f t="shared" si="4"/>
+        <v>10000</v>
       </c>
       <c r="P13" s="3" t="s">
         <v>10</v>
@@ -1795,16 +1800,16 @@
         <v>4</v>
       </c>
       <c r="J14" s="3">
-        <f>_xlfn.FLOOR.MATH(H14/$C$12)</f>
-        <v>100</v>
+        <f t="shared" si="5"/>
+        <v>5</v>
       </c>
       <c r="K14" s="5">
         <f t="shared" si="1"/>
-        <v>1.0000000000000009E-2</v>
+        <v>0.19999999999999996</v>
       </c>
       <c r="L14" s="3">
         <f t="shared" si="2"/>
-        <v>3200</v>
+        <v>160</v>
       </c>
       <c r="M14" s="3" t="s">
         <v>6</v>
@@ -1814,8 +1819,8 @@
         <v>1</v>
       </c>
       <c r="O14" s="3">
-        <f>1/($C$12*J14)</f>
-        <v>10000</v>
+        <f t="shared" si="4"/>
+        <v>20000</v>
       </c>
       <c r="P14" s="3" t="s">
         <v>10</v>
@@ -1836,16 +1841,16 @@
         <v>4</v>
       </c>
       <c r="J15" s="3">
-        <f>_xlfn.FLOOR.MATH(H15/$C$12)</f>
-        <v>55</v>
+        <f t="shared" si="5"/>
+        <v>2</v>
       </c>
       <c r="K15" s="5">
         <f t="shared" si="1"/>
-        <v>1.8181818181818188E-2</v>
+        <v>0.5</v>
       </c>
       <c r="L15" s="3">
         <f t="shared" si="2"/>
-        <v>1760</v>
+        <v>64</v>
       </c>
       <c r="M15" s="3" t="s">
         <v>6</v>
@@ -1855,8 +1860,8 @@
         <v>1</v>
       </c>
       <c r="O15" s="3">
-        <f>1/($C$12*J15)</f>
-        <v>18181.818181818184</v>
+        <f t="shared" si="4"/>
+        <v>49999.999999999993</v>
       </c>
       <c r="P15" s="3" t="s">
         <v>10</v>
@@ -1877,16 +1882,16 @@
         <v>4</v>
       </c>
       <c r="J16" s="3">
-        <f>_xlfn.FLOOR.MATH(H16/$C$12)</f>
-        <v>50</v>
+        <f t="shared" si="5"/>
+        <v>2</v>
       </c>
       <c r="K16" s="5">
         <f t="shared" si="1"/>
-        <v>2.0000000000000018E-2</v>
+        <v>0.5</v>
       </c>
       <c r="L16" s="3">
         <f t="shared" si="2"/>
-        <v>1600</v>
+        <v>64</v>
       </c>
       <c r="M16" s="3" t="s">
         <v>6</v>
@@ -1896,8 +1901,8 @@
         <v>1</v>
       </c>
       <c r="O16" s="3">
-        <f>1/($C$12*J16)</f>
-        <v>20000</v>
+        <f t="shared" si="4"/>
+        <v>49999.999999999993</v>
       </c>
       <c r="P16" s="3" t="s">
         <v>10</v>
@@ -1918,16 +1923,16 @@
         <v>4</v>
       </c>
       <c r="J17" s="3">
-        <f>_xlfn.FLOOR.MATH(H17/$C$12)</f>
-        <v>20</v>
+        <f t="shared" si="5"/>
+        <v>1</v>
       </c>
       <c r="K17" s="5">
         <f t="shared" si="1"/>
-        <v>5.0000000000000044E-2</v>
+        <v>1</v>
       </c>
       <c r="L17" s="3">
         <f t="shared" si="2"/>
-        <v>640</v>
+        <v>32</v>
       </c>
       <c r="M17" s="3" t="s">
         <v>6</v>
@@ -1937,8 +1942,8 @@
         <v>1</v>
       </c>
       <c r="O17" s="3">
-        <f>1/($C$12*J17)</f>
-        <v>50000.000000000007</v>
+        <f t="shared" si="4"/>
+        <v>99999.999999999985</v>
       </c>
       <c r="P17" s="3" t="s">
         <v>10</v>
@@ -1959,27 +1964,27 @@
         <v>4</v>
       </c>
       <c r="J18" s="3">
-        <f>_xlfn.FLOOR.MATH(H18/$C$12)</f>
-        <v>10</v>
-      </c>
-      <c r="K18" s="5">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="K18" s="5" t="e">
         <f t="shared" si="1"/>
-        <v>9.9999999999999978E-2</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="L18" s="3">
         <f t="shared" si="2"/>
-        <v>320</v>
+        <v>0</v>
       </c>
       <c r="M18" s="3" t="s">
         <v>6</v>
       </c>
       <c r="N18" s="3">
         <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="O18" s="3">
-        <f>1/($C$12*J18)</f>
-        <v>100000.00000000001</v>
+        <v>0</v>
+      </c>
+      <c r="O18" s="3" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
       </c>
       <c r="P18" s="3" t="s">
         <v>10</v>
@@ -2000,27 +2005,27 @@
         <v>4</v>
       </c>
       <c r="J19" s="3">
-        <f>_xlfn.FLOOR.MATH(H19/$C$12)</f>
-        <v>2</v>
-      </c>
-      <c r="K19" s="5">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="K19" s="5" t="e">
         <f t="shared" si="1"/>
-        <v>0.5</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="L19" s="3">
         <f t="shared" si="2"/>
-        <v>64</v>
+        <v>0</v>
       </c>
       <c r="M19" s="3" t="s">
         <v>6</v>
       </c>
       <c r="N19" s="3">
         <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="O19" s="3">
-        <f>1/($C$12*J19)</f>
-        <v>500000</v>
+        <v>0</v>
+      </c>
+      <c r="O19" s="3" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
       </c>
       <c r="P19" s="3" t="s">
         <v>10</v>

</xml_diff>

<commit_message>
updated pulse width limits + calc
</commit_message>
<xml_diff>
--- a/doc/dma_pwm_pulse_width_calculator.xlsx
+++ b/doc/dma_pwm_pulse_width_calculator.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ben\Documents\Projects\RT Robot\Documentation\Topics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B4D5F0A-1325-41DC-B27E-13C1AAB46A87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6EEA311-8E1A-4424-8AA5-52BF2DA59DBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="23940" yWindow="630" windowWidth="30195" windowHeight="14730" xr2:uid="{581135D7-DF17-4593-87AB-39E2EE409C02}"/>
+    <workbookView xWindow="18525" yWindow="2745" windowWidth="32295" windowHeight="18495" xr2:uid="{581135D7-DF17-4593-87AB-39E2EE409C02}"/>
   </bookViews>
   <sheets>
     <sheet name="Pulse Width" sheetId="1" r:id="rId1"/>
@@ -214,7 +214,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -248,9 +248,6 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="11" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -271,6 +268,15 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -589,7 +595,7 @@
   <dimension ref="B1:P19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -608,7 +614,7 @@
     <col min="12" max="12" width="9.140625" style="2"/>
     <col min="13" max="13" width="3.140625" style="2" customWidth="1"/>
     <col min="14" max="14" width="6.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="6" style="2" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.5703125" style="2" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="3.140625" style="2" bestFit="1" customWidth="1"/>
     <col min="17" max="16384" width="9.140625" style="2"/>
   </cols>
@@ -619,83 +625,83 @@
       <c r="D1" s="8"/>
     </row>
     <row r="2" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="17" t="s">
+      <c r="B2" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="17"/>
-      <c r="D2" s="17"/>
-      <c r="E2" s="17"/>
-      <c r="F2" s="17"/>
-      <c r="G2" s="17"/>
-      <c r="H2" s="17"/>
-      <c r="I2" s="17"/>
-      <c r="J2" s="17"/>
-      <c r="K2" s="17"/>
-      <c r="L2" s="19" t="s">
+      <c r="C2" s="16"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="16"/>
+      <c r="F2" s="16"/>
+      <c r="G2" s="16"/>
+      <c r="H2" s="16"/>
+      <c r="I2" s="16"/>
+      <c r="J2" s="16"/>
+      <c r="K2" s="16"/>
+      <c r="L2" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="M2" s="19"/>
-      <c r="N2" s="19"/>
-      <c r="O2" s="19"/>
-      <c r="P2" s="19"/>
+      <c r="M2" s="18"/>
+      <c r="N2" s="18"/>
+      <c r="O2" s="18"/>
+      <c r="P2" s="18"/>
     </row>
     <row r="3" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="18"/>
-      <c r="C3" s="18"/>
-      <c r="D3" s="18"/>
-      <c r="E3" s="18"/>
-      <c r="F3" s="18"/>
-      <c r="G3" s="18"/>
-      <c r="H3" s="18"/>
-      <c r="I3" s="18"/>
-      <c r="J3" s="18"/>
-      <c r="K3" s="18"/>
-      <c r="L3" s="20"/>
-      <c r="M3" s="20"/>
-      <c r="N3" s="20"/>
-      <c r="O3" s="20"/>
-      <c r="P3" s="20"/>
+      <c r="B3" s="17"/>
+      <c r="C3" s="17"/>
+      <c r="D3" s="17"/>
+      <c r="E3" s="17"/>
+      <c r="F3" s="17"/>
+      <c r="G3" s="17"/>
+      <c r="H3" s="17"/>
+      <c r="I3" s="17"/>
+      <c r="J3" s="17"/>
+      <c r="K3" s="17"/>
+      <c r="L3" s="19"/>
+      <c r="M3" s="19"/>
+      <c r="N3" s="19"/>
+      <c r="O3" s="19"/>
+      <c r="P3" s="19"/>
     </row>
     <row r="5" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="13">
+      <c r="C5" s="22">
+        <f>C6/(10^6)</f>
         <v>1.0000000000000001E-5</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="15" t="s">
+      <c r="F5" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="G5" s="16"/>
-      <c r="H5" s="15" t="s">
+      <c r="G5" s="15"/>
+      <c r="H5" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="I5" s="16"/>
+      <c r="I5" s="15"/>
       <c r="J5" s="12" t="s">
         <v>13</v>
       </c>
       <c r="K5" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="L5" s="15" t="s">
+      <c r="L5" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="M5" s="16"/>
+      <c r="M5" s="15"/>
       <c r="N5" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="O5" s="15" t="s">
+      <c r="O5" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="P5" s="16"/>
+      <c r="P5" s="15"/>
     </row>
     <row r="6" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B6" s="1"/>
-      <c r="C6" s="1">
-        <f>C5*10^6</f>
+      <c r="C6" s="7">
         <v>10</v>
       </c>
       <c r="D6" s="1" t="s">
@@ -733,9 +739,9 @@
         <f t="shared" ref="N6:N7" si="3">_xlfn.CEILING.MATH(L6/4096)</f>
         <v>7813</v>
       </c>
-      <c r="O6" s="3">
-        <f t="shared" ref="O6:O19" si="4">1/($C$5*J6)</f>
-        <v>0.1</v>
+      <c r="O6" s="20">
+        <f>1/($C$5*J6)/2</f>
+        <v>0.05</v>
       </c>
       <c r="P6" s="3" t="s">
         <v>10</v>
@@ -759,7 +765,7 @@
         <v>4</v>
       </c>
       <c r="J7" s="3">
-        <f t="shared" ref="J7:J19" si="5">_xlfn.FLOOR.MATH(H7/$C$5/2)</f>
+        <f t="shared" ref="J7:J19" si="4">_xlfn.FLOOR.MATH(H7/$C$5/2)</f>
         <v>500000</v>
       </c>
       <c r="K7" s="5">
@@ -777,9 +783,9 @@
         <f t="shared" si="3"/>
         <v>3907</v>
       </c>
-      <c r="O7" s="3">
-        <f t="shared" si="4"/>
-        <v>0.2</v>
+      <c r="O7" s="20">
+        <f t="shared" ref="O7:O19" si="5">1/($C$5*J7)/2</f>
+        <v>0.1</v>
       </c>
       <c r="P7" s="3" t="s">
         <v>10</v>
@@ -803,7 +809,7 @@
         <v>4</v>
       </c>
       <c r="J8" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>50000</v>
       </c>
       <c r="K8" s="5">
@@ -821,9 +827,9 @@
         <f t="shared" ref="N8:N16" si="9">_xlfn.CEILING.MATH(L8/4096)</f>
         <v>391</v>
       </c>
-      <c r="O8" s="3">
-        <f t="shared" si="4"/>
-        <v>2</v>
+      <c r="O8" s="20">
+        <f t="shared" si="5"/>
+        <v>1</v>
       </c>
       <c r="P8" s="3" t="s">
         <v>10</v>
@@ -847,7 +853,7 @@
         <v>4</v>
       </c>
       <c r="J9" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>5000</v>
       </c>
       <c r="K9" s="5">
@@ -865,9 +871,9 @@
         <f t="shared" si="9"/>
         <v>40</v>
       </c>
-      <c r="O9" s="3">
-        <f t="shared" si="4"/>
-        <v>20</v>
+      <c r="O9" s="20">
+        <f t="shared" si="5"/>
+        <v>10</v>
       </c>
       <c r="P9" s="3" t="s">
         <v>10</v>
@@ -891,7 +897,7 @@
         <v>4</v>
       </c>
       <c r="J10" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>1000</v>
       </c>
       <c r="K10" s="5">
@@ -909,9 +915,9 @@
         <f t="shared" si="9"/>
         <v>8</v>
       </c>
-      <c r="O10" s="3">
-        <f t="shared" si="4"/>
-        <v>100</v>
+      <c r="O10" s="20">
+        <f t="shared" si="5"/>
+        <v>50</v>
       </c>
       <c r="P10" s="3" t="s">
         <v>10</v>
@@ -935,7 +941,7 @@
         <v>4</v>
       </c>
       <c r="J11" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>500</v>
       </c>
       <c r="K11" s="5">
@@ -953,9 +959,9 @@
         <f t="shared" si="9"/>
         <v>4</v>
       </c>
-      <c r="O11" s="3">
-        <f t="shared" si="4"/>
-        <v>200</v>
+      <c r="O11" s="20">
+        <f t="shared" si="5"/>
+        <v>100</v>
       </c>
       <c r="P11" s="3" t="s">
         <v>10</v>
@@ -976,7 +982,7 @@
         <v>4</v>
       </c>
       <c r="J12" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>50</v>
       </c>
       <c r="K12" s="5">
@@ -994,9 +1000,9 @@
         <f t="shared" si="9"/>
         <v>1</v>
       </c>
-      <c r="O12" s="3">
-        <f t="shared" si="4"/>
-        <v>2000</v>
+      <c r="O12" s="20">
+        <f t="shared" si="5"/>
+        <v>1000</v>
       </c>
       <c r="P12" s="3" t="s">
         <v>10</v>
@@ -1017,7 +1023,7 @@
         <v>4</v>
       </c>
       <c r="J13" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>10</v>
       </c>
       <c r="K13" s="5">
@@ -1035,9 +1041,9 @@
         <f t="shared" si="9"/>
         <v>1</v>
       </c>
-      <c r="O13" s="3">
-        <f t="shared" si="4"/>
-        <v>10000</v>
+      <c r="O13" s="20">
+        <f t="shared" si="5"/>
+        <v>5000</v>
       </c>
       <c r="P13" s="3" t="s">
         <v>10</v>
@@ -1058,7 +1064,7 @@
         <v>4</v>
       </c>
       <c r="J14" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>5</v>
       </c>
       <c r="K14" s="5">
@@ -1076,9 +1082,9 @@
         <f t="shared" si="9"/>
         <v>1</v>
       </c>
-      <c r="O14" s="3">
-        <f t="shared" si="4"/>
-        <v>20000</v>
+      <c r="O14" s="20">
+        <f t="shared" si="5"/>
+        <v>10000</v>
       </c>
       <c r="P14" s="3" t="s">
         <v>10</v>
@@ -1099,7 +1105,7 @@
         <v>4</v>
       </c>
       <c r="J15" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="K15" s="5">
@@ -1117,9 +1123,9 @@
         <f t="shared" si="9"/>
         <v>1</v>
       </c>
-      <c r="O15" s="3">
-        <f t="shared" si="4"/>
-        <v>49999.999999999993</v>
+      <c r="O15" s="20">
+        <f t="shared" si="5"/>
+        <v>24999.999999999996</v>
       </c>
       <c r="P15" s="3" t="s">
         <v>10</v>
@@ -1140,7 +1146,7 @@
         <v>4</v>
       </c>
       <c r="J16" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="K16" s="5">
@@ -1158,9 +1164,9 @@
         <f t="shared" si="9"/>
         <v>1</v>
       </c>
-      <c r="O16" s="3">
-        <f t="shared" si="4"/>
-        <v>49999.999999999993</v>
+      <c r="O16" s="20">
+        <f t="shared" si="5"/>
+        <v>24999.999999999996</v>
       </c>
       <c r="P16" s="3" t="s">
         <v>10</v>
@@ -1181,7 +1187,7 @@
         <v>4</v>
       </c>
       <c r="J17" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="K17" s="5">
@@ -1199,9 +1205,9 @@
         <f t="shared" ref="N17:N19" si="13">_xlfn.CEILING.MATH(L17/4096)</f>
         <v>1</v>
       </c>
-      <c r="O17" s="3">
-        <f t="shared" si="4"/>
-        <v>99999.999999999985</v>
+      <c r="O17" s="20">
+        <f t="shared" si="5"/>
+        <v>49999.999999999993</v>
       </c>
       <c r="P17" s="3" t="s">
         <v>10</v>
@@ -1222,7 +1228,7 @@
         <v>4</v>
       </c>
       <c r="J18" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K18" s="5" t="e">
@@ -1240,8 +1246,8 @@
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
-      <c r="O18" s="3" t="e">
-        <f t="shared" si="4"/>
+      <c r="O18" s="20" t="e">
+        <f t="shared" si="5"/>
         <v>#DIV/0!</v>
       </c>
       <c r="P18" s="3" t="s">
@@ -1263,7 +1269,7 @@
         <v>4</v>
       </c>
       <c r="J19" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K19" s="5" t="e">
@@ -1281,8 +1287,8 @@
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
-      <c r="O19" s="3" t="e">
-        <f t="shared" si="4"/>
+      <c r="O19" s="20" t="e">
+        <f t="shared" si="5"/>
         <v>#DIV/0!</v>
       </c>
       <c r="P19" s="3" t="s">
@@ -1308,7 +1314,7 @@
   <dimension ref="B2:P19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1327,48 +1333,48 @@
     <col min="12" max="12" width="9.140625" style="2"/>
     <col min="13" max="13" width="3.140625" style="2" customWidth="1"/>
     <col min="14" max="14" width="6.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="6" style="2" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="8.28515625" style="2" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="3.140625" style="2" bestFit="1" customWidth="1"/>
     <col min="17" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B2" s="17" t="s">
+      <c r="B2" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="17"/>
-      <c r="D2" s="17"/>
-      <c r="E2" s="17"/>
-      <c r="F2" s="17"/>
-      <c r="G2" s="17"/>
-      <c r="H2" s="17"/>
-      <c r="I2" s="17"/>
-      <c r="J2" s="17"/>
-      <c r="K2" s="17"/>
-      <c r="L2" s="19" t="s">
+      <c r="C2" s="16"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="16"/>
+      <c r="F2" s="16"/>
+      <c r="G2" s="16"/>
+      <c r="H2" s="16"/>
+      <c r="I2" s="16"/>
+      <c r="J2" s="16"/>
+      <c r="K2" s="16"/>
+      <c r="L2" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="M2" s="19"/>
-      <c r="N2" s="19"/>
-      <c r="O2" s="19"/>
-      <c r="P2" s="19"/>
+      <c r="M2" s="18"/>
+      <c r="N2" s="18"/>
+      <c r="O2" s="18"/>
+      <c r="P2" s="18"/>
     </row>
     <row r="3" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B3" s="18"/>
-      <c r="C3" s="18"/>
-      <c r="D3" s="18"/>
-      <c r="E3" s="18"/>
-      <c r="F3" s="18"/>
-      <c r="G3" s="18"/>
-      <c r="H3" s="18"/>
-      <c r="I3" s="18"/>
-      <c r="J3" s="18"/>
-      <c r="K3" s="18"/>
-      <c r="L3" s="20"/>
-      <c r="M3" s="20"/>
-      <c r="N3" s="20"/>
-      <c r="O3" s="20"/>
-      <c r="P3" s="20"/>
+      <c r="B3" s="17"/>
+      <c r="C3" s="17"/>
+      <c r="D3" s="17"/>
+      <c r="E3" s="17"/>
+      <c r="F3" s="17"/>
+      <c r="G3" s="17"/>
+      <c r="H3" s="17"/>
+      <c r="I3" s="17"/>
+      <c r="J3" s="17"/>
+      <c r="K3" s="17"/>
+      <c r="L3" s="19"/>
+      <c r="M3" s="19"/>
+      <c r="N3" s="19"/>
+      <c r="O3" s="19"/>
+      <c r="P3" s="19"/>
     </row>
     <row r="5" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
@@ -1380,31 +1386,31 @@
       <c r="D5" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="F5" s="15" t="s">
+      <c r="F5" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="G5" s="16"/>
-      <c r="H5" s="15" t="s">
+      <c r="G5" s="15"/>
+      <c r="H5" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="I5" s="16"/>
+      <c r="I5" s="15"/>
       <c r="J5" s="12" t="s">
         <v>13</v>
       </c>
       <c r="K5" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="L5" s="15" t="s">
+      <c r="L5" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="M5" s="16"/>
+      <c r="M5" s="15"/>
       <c r="N5" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="O5" s="15" t="s">
+      <c r="O5" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="P5" s="16"/>
+      <c r="P5" s="15"/>
     </row>
     <row r="6" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
@@ -1446,9 +1452,9 @@
         <f t="shared" ref="N6:N19" si="3">_xlfn.CEILING.MATH(L6/4096)</f>
         <v>7813</v>
       </c>
-      <c r="O6" s="3">
-        <f t="shared" ref="O6:O19" si="4">1/($C$12*J6)</f>
-        <v>0.1</v>
+      <c r="O6" s="21">
+        <f>1/($C$12*J6)/2</f>
+        <v>0.05</v>
       </c>
       <c r="P6" s="3" t="s">
         <v>10</v>
@@ -1472,7 +1478,7 @@
         <v>4</v>
       </c>
       <c r="J7" s="3">
-        <f t="shared" ref="J7:J19" si="5">_xlfn.FLOOR.MATH(H7/$C$12/2)</f>
+        <f t="shared" ref="J7:J19" si="4">_xlfn.FLOOR.MATH(H7/$C$12/2)</f>
         <v>500000</v>
       </c>
       <c r="K7" s="5">
@@ -1490,9 +1496,9 @@
         <f t="shared" si="3"/>
         <v>3907</v>
       </c>
-      <c r="O7" s="3">
-        <f t="shared" si="4"/>
-        <v>0.2</v>
+      <c r="O7" s="21">
+        <f t="shared" ref="O7:O19" si="5">1/($C$12*J7)/2</f>
+        <v>0.1</v>
       </c>
       <c r="P7" s="3" t="s">
         <v>10</v>
@@ -1523,7 +1529,7 @@
         <v>4</v>
       </c>
       <c r="J8" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>50000</v>
       </c>
       <c r="K8" s="5">
@@ -1541,9 +1547,9 @@
         <f t="shared" si="3"/>
         <v>391</v>
       </c>
-      <c r="O8" s="3">
-        <f t="shared" si="4"/>
-        <v>2</v>
+      <c r="O8" s="21">
+        <f t="shared" si="5"/>
+        <v>1</v>
       </c>
       <c r="P8" s="3" t="s">
         <v>10</v>
@@ -1571,7 +1577,7 @@
         <v>4</v>
       </c>
       <c r="J9" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>5000</v>
       </c>
       <c r="K9" s="5">
@@ -1589,9 +1595,9 @@
         <f t="shared" si="3"/>
         <v>40</v>
       </c>
-      <c r="O9" s="3">
-        <f t="shared" si="4"/>
-        <v>20</v>
+      <c r="O9" s="21">
+        <f t="shared" si="5"/>
+        <v>10</v>
       </c>
       <c r="P9" s="3" t="s">
         <v>10</v>
@@ -1615,7 +1621,7 @@
         <v>4</v>
       </c>
       <c r="J10" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>1000</v>
       </c>
       <c r="K10" s="5">
@@ -1633,9 +1639,9 @@
         <f t="shared" si="3"/>
         <v>8</v>
       </c>
-      <c r="O10" s="3">
-        <f t="shared" si="4"/>
-        <v>100</v>
+      <c r="O10" s="21">
+        <f t="shared" si="5"/>
+        <v>50</v>
       </c>
       <c r="P10" s="3" t="s">
         <v>10</v>
@@ -1659,7 +1665,7 @@
         <v>4</v>
       </c>
       <c r="J11" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>500</v>
       </c>
       <c r="K11" s="5">
@@ -1677,9 +1683,9 @@
         <f t="shared" si="3"/>
         <v>4</v>
       </c>
-      <c r="O11" s="3">
-        <f t="shared" si="4"/>
-        <v>200</v>
+      <c r="O11" s="21">
+        <f t="shared" si="5"/>
+        <v>100</v>
       </c>
       <c r="P11" s="3" t="s">
         <v>10</v>
@@ -1689,7 +1695,7 @@
       <c r="B12" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C12" s="14">
+      <c r="C12" s="13">
         <f>C9/(C8*10^6)</f>
         <v>1.0000000000000001E-5</v>
       </c>
@@ -1710,7 +1716,7 @@
         <v>4</v>
       </c>
       <c r="J12" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>50</v>
       </c>
       <c r="K12" s="5">
@@ -1728,9 +1734,9 @@
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="O12" s="3">
-        <f t="shared" si="4"/>
-        <v>2000</v>
+      <c r="O12" s="21">
+        <f t="shared" si="5"/>
+        <v>1000</v>
       </c>
       <c r="P12" s="3" t="s">
         <v>10</v>
@@ -1759,7 +1765,7 @@
         <v>4</v>
       </c>
       <c r="J13" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>10</v>
       </c>
       <c r="K13" s="5">
@@ -1777,9 +1783,9 @@
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="O13" s="3">
-        <f t="shared" si="4"/>
-        <v>10000</v>
+      <c r="O13" s="21">
+        <f t="shared" si="5"/>
+        <v>5000</v>
       </c>
       <c r="P13" s="3" t="s">
         <v>10</v>
@@ -1800,7 +1806,7 @@
         <v>4</v>
       </c>
       <c r="J14" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>5</v>
       </c>
       <c r="K14" s="5">
@@ -1818,9 +1824,9 @@
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="O14" s="3">
-        <f t="shared" si="4"/>
-        <v>20000</v>
+      <c r="O14" s="21">
+        <f t="shared" si="5"/>
+        <v>10000</v>
       </c>
       <c r="P14" s="3" t="s">
         <v>10</v>
@@ -1841,7 +1847,7 @@
         <v>4</v>
       </c>
       <c r="J15" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="K15" s="5">
@@ -1859,9 +1865,9 @@
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="O15" s="3">
-        <f t="shared" si="4"/>
-        <v>49999.999999999993</v>
+      <c r="O15" s="21">
+        <f t="shared" si="5"/>
+        <v>24999.999999999996</v>
       </c>
       <c r="P15" s="3" t="s">
         <v>10</v>
@@ -1882,7 +1888,7 @@
         <v>4</v>
       </c>
       <c r="J16" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="K16" s="5">
@@ -1900,9 +1906,9 @@
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="O16" s="3">
-        <f t="shared" si="4"/>
-        <v>49999.999999999993</v>
+      <c r="O16" s="21">
+        <f t="shared" si="5"/>
+        <v>24999.999999999996</v>
       </c>
       <c r="P16" s="3" t="s">
         <v>10</v>
@@ -1923,7 +1929,7 @@
         <v>4</v>
       </c>
       <c r="J17" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="K17" s="5">
@@ -1941,9 +1947,9 @@
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="O17" s="3">
-        <f t="shared" si="4"/>
-        <v>99999.999999999985</v>
+      <c r="O17" s="21">
+        <f t="shared" si="5"/>
+        <v>49999.999999999993</v>
       </c>
       <c r="P17" s="3" t="s">
         <v>10</v>
@@ -1964,7 +1970,7 @@
         <v>4</v>
       </c>
       <c r="J18" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K18" s="5" t="e">
@@ -1982,8 +1988,8 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="O18" s="3" t="e">
-        <f t="shared" si="4"/>
+      <c r="O18" s="21" t="e">
+        <f t="shared" si="5"/>
         <v>#DIV/0!</v>
       </c>
       <c r="P18" s="3" t="s">
@@ -2005,7 +2011,7 @@
         <v>4</v>
       </c>
       <c r="J19" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K19" s="5" t="e">
@@ -2023,8 +2029,8 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="O19" s="3" t="e">
-        <f t="shared" si="4"/>
+      <c r="O19" s="21" t="e">
+        <f t="shared" si="5"/>
         <v>#DIV/0!</v>
       </c>
       <c r="P19" s="3" t="s">

</xml_diff>